<commit_message>
Updates all sales and marketing data
</commit_message>
<xml_diff>
--- a/prototype_data.xlsx
+++ b/prototype_data.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8900" yWindow="1600" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="8900" yWindow="1600" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" r:id="rId1"/>
-    <sheet name="Marketing Impressions" sheetId="2" r:id="rId2"/>
+    <sheet name="Marketing Spend" sheetId="2" r:id="rId2"/>
     <sheet name="Dashboard Charts" sheetId="3" r:id="rId3"/>
     <sheet name="Portfolio Investment" sheetId="4" r:id="rId4"/>
+    <sheet name="Sales&amp;Marketing" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Twitter</t>
   </si>
@@ -36,9 +37,6 @@
     <t>Month</t>
   </si>
   <si>
-    <t>Sales</t>
-  </si>
-  <si>
     <t>Fund Investment</t>
   </si>
   <si>
@@ -49,6 +47,12 @@
   </si>
   <si>
     <t>Melindas Investments</t>
+  </si>
+  <si>
+    <t>Sales Revenue</t>
+  </si>
+  <si>
+    <t>Marketing Spend</t>
   </si>
 </sst>
 </file>
@@ -97,7 +101,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -129,12 +133,77 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -150,6 +219,38 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -165,6 +266,38 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -197,7 +330,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Marketing Impressions'!$B$1</c:f>
+              <c:f>'Marketing Spend'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -211,7 +344,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Marketing Impressions'!$A$1:$A$25</c:f>
+              <c:f>'Marketing Spend'!$A$1:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
@@ -294,81 +427,81 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Marketing Impressions'!$B$2:$B$25</c:f>
+              <c:f>'Marketing Spend'!$B$2:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.0</c:v>
+                  <c:v>700.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50.0</c:v>
+                  <c:v>2500.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70.0</c:v>
+                  <c:v>3500.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>110.0</c:v>
+                  <c:v>5500.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>110.0</c:v>
+                  <c:v>5500.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>115.0</c:v>
+                  <c:v>5750.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>120.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>140.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>200.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>210.0</c:v>
+                  <c:v>10500.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>300.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>350.0</c:v>
+                  <c:v>17500.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>360.0</c:v>
+                  <c:v>18000.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>380.0</c:v>
+                  <c:v>19000.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>380.0</c:v>
+                  <c:v>19000.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>400.0</c:v>
+                  <c:v>20000.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>410.0</c:v>
+                  <c:v>20500.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>420.0</c:v>
+                  <c:v>21000.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>440.0</c:v>
+                  <c:v>22000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -380,7 +513,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Marketing Impressions'!$C$1</c:f>
+              <c:f>'Marketing Spend'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -394,7 +527,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Marketing Impressions'!$A$1:$A$25</c:f>
+              <c:f>'Marketing Spend'!$A$1:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
@@ -477,81 +610,81 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Marketing Impressions'!$C$2:$C$25</c:f>
+              <c:f>'Marketing Spend'!$C$2:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>20.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.0</c:v>
+                  <c:v>1400.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>3500.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>85.0</c:v>
+                  <c:v>4250.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90.0</c:v>
+                  <c:v>4500.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>140.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>160.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>180.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>180.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>220.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>240.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>255.0</c:v>
+                  <c:v>12750.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>260.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>280.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>310.0</c:v>
+                  <c:v>15500.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>320.0</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>340.0</c:v>
+                  <c:v>17000.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>460.0</c:v>
+                  <c:v>23000.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>500.0</c:v>
+                  <c:v>25000.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>580.0</c:v>
+                  <c:v>29000.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>630.0</c:v>
+                  <c:v>31500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -563,7 +696,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Marketing Impressions'!$D$1</c:f>
+              <c:f>'Marketing Spend'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -577,7 +710,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Marketing Impressions'!$A$1:$A$25</c:f>
+              <c:f>'Marketing Spend'!$A$1:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
@@ -660,81 +793,81 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Marketing Impressions'!$D$2:$D$25</c:f>
+              <c:f>'Marketing Spend'!$D$2:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>250.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.0</c:v>
+                  <c:v>750.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.0</c:v>
+                  <c:v>1200.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.0</c:v>
+                  <c:v>1500.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45.0</c:v>
+                  <c:v>2250.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50.0</c:v>
+                  <c:v>2500.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>60.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>65.0</c:v>
+                  <c:v>3250.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>65.0</c:v>
+                  <c:v>3250.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>65.0</c:v>
+                  <c:v>3250.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45.0</c:v>
+                  <c:v>2250.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>55.0</c:v>
+                  <c:v>2750.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>60.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75.0</c:v>
+                  <c:v>3750.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>80.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>75.0</c:v>
+                  <c:v>3750.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>68.0</c:v>
+                  <c:v>3400.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>80.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>95.0</c:v>
+                  <c:v>4750.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>100.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>110.0</c:v>
+                  <c:v>5500.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>120.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -797,6 +930,13 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:alpha val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
@@ -945,76 +1085,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1500.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>7500.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.0</c:v>
+                  <c:v>22500.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.0</c:v>
+                  <c:v>25500.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.0</c:v>
+                  <c:v>27000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.0</c:v>
+                  <c:v>45000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.0</c:v>
+                  <c:v>52500.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33.0</c:v>
+                  <c:v>49500.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40.0</c:v>
+                  <c:v>60000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60.0</c:v>
+                  <c:v>90000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>70.0</c:v>
+                  <c:v>105000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>75.0</c:v>
+                  <c:v>112500.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>75.0</c:v>
+                  <c:v>112500.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>80.0</c:v>
+                  <c:v>120000.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>90.0</c:v>
+                  <c:v>135000.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>95.0</c:v>
+                  <c:v>142500.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>110.0</c:v>
+                  <c:v>165000.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>115.0</c:v>
+                  <c:v>172500.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>130.0</c:v>
+                  <c:v>195000.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>135.0</c:v>
+                  <c:v>202500.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>160.0</c:v>
+                  <c:v>240000.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>180.0</c:v>
+                  <c:v>270000.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>220.0</c:v>
+                  <c:v>330000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1155,10 +1295,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.6</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1176,6 +1316,321 @@
         <c:firstSliceAng val="0"/>
         <c:holeSize val="50"/>
       </c:doughnutChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:alpha val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1">
+        <a:alpha val="40000"/>
+      </a:schemeClr>
+    </a:solidFill>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sales&amp;Marketing'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sales Revenue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sales&amp;Marketing'!$A$2:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>49500.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60000.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>112500.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>112500.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>120000.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>135000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>142500.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>165000.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>172500.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>195000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>202500.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>240000.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>270000.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>330000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sales&amp;Marketing'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Marketing Spend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sales&amp;Marketing'!$B$2:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1750.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2850.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7200.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9250.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10750.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15500.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16750.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18250.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20250.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24750.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26250.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31750.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>35500.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>37250.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38400.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>47750.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>50500.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>55500.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>59500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2067876680"/>
+        <c:axId val="-2065676712"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2067876680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2065676712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2065676712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2067876680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:alpha val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
@@ -1291,6 +1746,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1633,7 +2123,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+      <selection activeCell="B1" sqref="B1:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1643,7 +2133,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1651,7 +2141,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1659,7 +2149,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1667,7 +2157,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1675,7 +2165,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>22500</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1683,7 +2173,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>25500</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1691,7 +2181,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>18</v>
+        <v>27000</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1699,7 +2189,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>30</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1707,7 +2197,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>35</v>
+        <v>52500</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1715,7 +2205,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>33</v>
+        <v>49500</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1723,7 +2213,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>40</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1731,7 +2221,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>60</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1739,7 +2229,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>70</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1747,7 +2237,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>75</v>
+        <v>112500</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1755,7 +2245,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>75</v>
+        <v>112500</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1763,7 +2253,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1771,7 +2261,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>90</v>
+        <v>135000</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1779,7 +2269,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>95</v>
+        <v>142500</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1787,7 +2277,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>110</v>
+        <v>165000</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1795,7 +2285,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>115</v>
+        <v>172500</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1803,7 +2293,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>130</v>
+        <v>195000</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1811,7 +2301,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>135</v>
+        <v>202500</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1819,7 +2309,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>160</v>
+        <v>240000</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1827,7 +2317,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>180</v>
+        <v>270000</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1835,11 +2325,12 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>220</v>
+        <v>330000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1850,15 +2341,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1871,345 +2362,451 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>500</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="D2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>250</v>
+      </c>
+      <c r="E2">
+        <f>B2+C2+D2</f>
+        <v>1750</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>700</v>
       </c>
       <c r="C3">
-        <v>28</v>
+        <v>1400</v>
       </c>
       <c r="D3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>750</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E25" si="0">B3+C3+D3</f>
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>2000</v>
       </c>
       <c r="C4">
-        <v>60</v>
+        <v>3000</v>
       </c>
       <c r="D4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>50</v>
+        <v>2500</v>
       </c>
       <c r="C5">
-        <v>70</v>
+        <v>3500</v>
       </c>
       <c r="D5">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>1200</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>70</v>
+        <v>3500</v>
       </c>
       <c r="C6">
-        <v>80</v>
+        <v>4000</v>
       </c>
       <c r="D6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>1500</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>9000</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>60</v>
+        <v>3000</v>
       </c>
       <c r="C7">
-        <v>85</v>
+        <v>4250</v>
       </c>
       <c r="D7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>2000</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>9250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>80</v>
+        <v>4000</v>
       </c>
       <c r="C8">
-        <v>90</v>
+        <v>4500</v>
       </c>
       <c r="D8">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>2250</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>10750</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="C9">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="D9">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>2500</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>110</v>
+        <v>5500</v>
       </c>
       <c r="C10">
-        <v>140</v>
+        <v>7000</v>
       </c>
       <c r="D10">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>3000</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>15500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>110</v>
+        <v>5500</v>
       </c>
       <c r="C11">
-        <v>160</v>
+        <v>8000</v>
       </c>
       <c r="D11">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>3250</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>16750</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>115</v>
+        <v>5750</v>
       </c>
       <c r="C12">
-        <v>180</v>
+        <v>9000</v>
       </c>
       <c r="D12">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>3250</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>120</v>
+        <v>6000</v>
       </c>
       <c r="C13">
-        <v>180</v>
+        <v>9000</v>
       </c>
       <c r="D13">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>3250</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>18250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>140</v>
+        <v>7000</v>
       </c>
       <c r="C14">
-        <v>220</v>
+        <v>11000</v>
       </c>
       <c r="D14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>2250</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>20250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>200</v>
+        <v>10000</v>
       </c>
       <c r="C15">
-        <v>240</v>
+        <v>12000</v>
       </c>
       <c r="D15">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>2750</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>24750</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>210</v>
+        <v>10500</v>
       </c>
       <c r="C16">
-        <v>255</v>
+        <v>12750</v>
       </c>
       <c r="D16">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>3000</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>26250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>300</v>
+        <v>15000</v>
       </c>
       <c r="C17">
-        <v>260</v>
+        <v>13000</v>
       </c>
       <c r="D17">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>3750</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>31750</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>350</v>
+        <v>17500</v>
       </c>
       <c r="C18">
-        <v>280</v>
+        <v>14000</v>
       </c>
       <c r="D18">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>4000</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>35500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>360</v>
+        <v>18000</v>
       </c>
       <c r="C19">
-        <v>310</v>
+        <v>15500</v>
       </c>
       <c r="D19">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>3750</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>37250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>380</v>
+        <v>19000</v>
       </c>
       <c r="C20">
-        <v>320</v>
+        <v>16000</v>
       </c>
       <c r="D20">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>3400</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>38400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>380</v>
+        <v>19000</v>
       </c>
       <c r="C21">
-        <v>340</v>
+        <v>17000</v>
       </c>
       <c r="D21">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>4000</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>400</v>
+        <v>20000</v>
       </c>
       <c r="C22">
-        <v>460</v>
+        <v>23000</v>
       </c>
       <c r="D22">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>4750</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>47750</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>410</v>
+        <v>20500</v>
       </c>
       <c r="C23">
-        <v>500</v>
+        <v>25000</v>
       </c>
       <c r="D23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>5000</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>50500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>420</v>
+        <v>21000</v>
       </c>
       <c r="C24">
-        <v>580</v>
+        <v>29000</v>
       </c>
       <c r="D24">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>5500</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>55500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>440</v>
+        <v>22000</v>
       </c>
       <c r="C25">
-        <v>630</v>
+        <v>31500</v>
       </c>
       <c r="D25">
-        <v>120</v>
+        <v>6000</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>59500</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2223,7 +2820,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2242,34 +2839,259 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1">
-        <v>0.4</v>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1500</v>
+      </c>
+      <c r="B2">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>7500</v>
+      </c>
+      <c r="B3">
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>15000</v>
+      </c>
+      <c r="B4">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>22500</v>
+      </c>
+      <c r="B5">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>25500</v>
+      </c>
+      <c r="B6">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>27000</v>
+      </c>
+      <c r="B7">
+        <v>9250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>45000</v>
+      </c>
+      <c r="B8">
+        <v>10750</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>52500</v>
+      </c>
+      <c r="B9">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>49500</v>
+      </c>
+      <c r="B10">
+        <v>15500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>60000</v>
+      </c>
+      <c r="B11">
+        <v>16750</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>90000</v>
+      </c>
+      <c r="B12">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>105000</v>
+      </c>
+      <c r="B13">
+        <v>18250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>112500</v>
+      </c>
+      <c r="B14">
+        <v>20250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>112500</v>
+      </c>
+      <c r="B15">
+        <v>24750</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>120000</v>
+      </c>
+      <c r="B16">
+        <v>26250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>135000</v>
+      </c>
+      <c r="B17">
+        <v>31750</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>142500</v>
+      </c>
+      <c r="B18">
+        <v>35500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>165000</v>
+      </c>
+      <c r="B19">
+        <v>37250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>172500</v>
+      </c>
+      <c r="B20">
+        <v>38400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>195000</v>
+      </c>
+      <c r="B21">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>202500</v>
+      </c>
+      <c r="B22">
+        <v>47750</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>240000</v>
+      </c>
+      <c r="B23">
+        <v>50500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>270000</v>
+      </c>
+      <c r="B24">
+        <v>55500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>330000</v>
+      </c>
+      <c r="B25">
+        <v>59500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds portfolio recurring return graph
</commit_message>
<xml_diff>
--- a/prototype_data.xlsx
+++ b/prototype_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8900" yWindow="1600" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="8900" yWindow="1600" windowWidth="25600" windowHeight="19020" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Dashboard Charts" sheetId="3" r:id="rId3"/>
     <sheet name="Portfolio Investment" sheetId="4" r:id="rId4"/>
     <sheet name="Sales&amp;Marketing" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Twitter</t>
   </si>
@@ -53,6 +54,9 @@
   </si>
   <si>
     <t>Marketing Spend</t>
+  </si>
+  <si>
+    <t>Return</t>
   </si>
 </sst>
 </file>
@@ -1663,6 +1667,224 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet6!$B$2:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1400.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15000.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30000.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60000.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>65000.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>55000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>57000.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>70000.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>85000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90000.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>102000.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>99000.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>105000.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>120000.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>140000.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>170000.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>200000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>240000.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>230000.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>260000.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>300000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320000.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>340000.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>380000.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>400000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2048135864"/>
+        <c:axId val="-2051673112"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2048135864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2051673112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2051673112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2048135864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:alpha val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1">
+        <a:alpha val="40000"/>
+      </a:schemeClr>
+    </a:solidFill>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1781,6 +2003,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2885,7 +3142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -3104,4 +3361,321 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>57000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>85000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>102000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>99000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>230000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>260000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>320000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>340000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>380000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>400000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>